<commit_message>
Code calculates emissions for all Reisen/Wege
Changes include:
- new input files: I created separate excel sheets for UBA and HBEFA data
- changed the code to use UBA data and complete missing values with HBEFA data
This code calculates emissions for all Reisen/Wege with now very few NAs (corresponding to Schiff and Andere/Keine Angabe)
Ready for aggregation at the individual level!
</commit_message>
<xml_diff>
--- a/Mobility_data/Other_input/hvm_diff2_matching.xlsx
+++ b/Mobility_data/Other_input/hvm_diff2_matching.xlsx
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>